<commit_message>
tabel met berekening min en max kosten naar .py
</commit_message>
<xml_diff>
--- a/calculations/tabel uit opdracht.xlsx
+++ b/calculations/tabel uit opdracht.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebecca\Documents\UvA\Minor Programmeren\Heuristieken\CargoLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebecca\Documents\UvA\Minor_Programmeren\Heuristieken\github\heuristieken\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA88EAB-29F2-474F-AF89-2E3F0844651B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D20952B-467C-4A8A-98E0-FE872152EB71}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6670" xr2:uid="{A3E26F79-F5C0-4F7D-93C9-45C4392BA124}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,16 +553,16 @@
         <v>0.73</v>
       </c>
       <c r="J2">
-        <f>F2*H2</f>
-        <v>5402</v>
+        <f>F2*H2 / (1-H2)</f>
+        <v>20007.407407407405</v>
       </c>
       <c r="K2">
-        <f>J2*1000*5</f>
-        <v>27010000</v>
+        <f>ROUNDUP(J2*1000, 0)*5</f>
+        <v>100037040</v>
       </c>
       <c r="M2">
         <f>K2+G2</f>
-        <v>417010000</v>
+        <v>490037040</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -591,16 +591,16 @@
         <v>0.74</v>
       </c>
       <c r="J3">
-        <f>F3*H3</f>
-        <v>5194.8</v>
+        <f t="shared" ref="J3:J6" si="0">F3*H3 / (1-H3)</f>
+        <v>19980</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K6" si="0">J3*1000*5</f>
-        <v>25974000</v>
+        <f t="shared" ref="K3:K5" si="1">ROUNDUP(J3*1000, 0)*5</f>
+        <v>99900000</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M5" si="1">K3+G3</f>
-        <v>200974000</v>
+        <f t="shared" ref="M3:M5" si="2">K3+G3</f>
+        <v>274900000</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -629,16 +629,16 @@
         <v>0.71</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J5" si="2">F4*H4</f>
-        <v>7455</v>
+        <f t="shared" si="0"/>
+        <v>25706.896551724134</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>37275000</v>
+        <f t="shared" si="1"/>
+        <v>128534485</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
-        <v>457275000</v>
+        <f t="shared" si="2"/>
+        <v>548534485</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -667,16 +667,16 @@
         <v>0.72</v>
       </c>
       <c r="J5">
+        <f t="shared" si="0"/>
+        <v>31371.428571428569</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>156857145</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="2"/>
-        <v>8784</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>43920000</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
-        <v>390920000</v>
+        <v>503857145</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -684,16 +684,16 @@
         <v>22</v>
       </c>
       <c r="J6">
-        <f>SUM(J2:J5)</f>
-        <v>26835.8</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>134179000</v>
+        <f t="shared" ref="K3:K6" si="3">J6*1000*5</f>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
         <f>SUM(M2:M5)</f>
-        <v>1466179000</v>
+        <v>1817328670</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -709,58 +709,58 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J8">
-        <f>D2*H2</f>
-        <v>1460</v>
+        <f t="shared" ref="J8:J11" si="4">(D2 + F2)*H2 / (1-H2)</f>
+        <v>25414.814814814814</v>
       </c>
       <c r="K8">
-        <f>J8*1000*5</f>
-        <v>7300000</v>
+        <f>ROUNDUP(J8*1000, 0)*5</f>
+        <v>127074075</v>
       </c>
       <c r="M8">
-        <f>K8+M2</f>
-        <v>424310000</v>
+        <f>K8+G2</f>
+        <v>517074075</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J9">
-        <f>D3*H3</f>
-        <v>1776</v>
+        <f>(D3 + F3)*H3 / (1-H3)</f>
+        <v>26810.76923076923</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K11" si="3">J9*1000*5</f>
-        <v>8880000</v>
+        <f t="shared" ref="K9:K11" si="5">ROUNDUP(J9*1000, 0)*5</f>
+        <v>134053850</v>
       </c>
       <c r="M9">
-        <f>K9+M3</f>
-        <v>209854000</v>
+        <f t="shared" ref="M9:M11" si="6">K9+G3</f>
+        <v>309053850</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J10">
-        <f>D4*H4</f>
-        <v>3692</v>
+        <f t="shared" si="4"/>
+        <v>38437.931034482754</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>18460000</v>
+        <f t="shared" si="5"/>
+        <v>192189660</v>
       </c>
       <c r="M10">
-        <f>K10+M4</f>
-        <v>475735000</v>
+        <f t="shared" si="6"/>
+        <v>612189660</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J11">
-        <f>D5*H5</f>
-        <v>4320</v>
+        <f t="shared" si="4"/>
+        <v>46799.999999999993</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
-        <v>21600000</v>
+        <f t="shared" si="5"/>
+        <v>234000000</v>
       </c>
       <c r="M11">
-        <f>K11+M5</f>
-        <v>412520000</v>
+        <f t="shared" si="6"/>
+        <v>581000000</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -769,11 +769,11 @@
       </c>
       <c r="K12">
         <f>SUM(K8:K11)</f>
-        <v>56240000</v>
+        <v>687317585</v>
       </c>
       <c r="M12" s="2">
         <f>SUM(M8:M11)</f>
-        <v>1522419000</v>
+        <v>2019317585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>